<commit_message>
finalized processing of data set
</commit_message>
<xml_diff>
--- a/code/processing/growth_curves_plate_reader/20201021_r1_O2_ST_tetracycline_sucrose_test/20201021_plate_layout.xlsx
+++ b/code/processing/growth_curves_plate_reader/20201021_r1_O2_ST_tetracycline_sucrose_test/20201021_plate_layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomroschinger/git/evo_mwc/code/processing/growth_curves_plate_reader/20201021_r1_O2_ST_tetracycline_sucrose_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04EC977-68B3-1F40-98C4-5B25BF768D4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5763A27-D8BC-AE4B-8A33-58776CE81498}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42340" yWindow="-12880" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -742,34 +742,34 @@
         <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="H2" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="I2" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="J2" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="K2" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="L2" t="s">
         <v>81</v>
@@ -780,34 +780,34 @@
         <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="G3" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="H3" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="I3" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="J3" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="K3" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="L3" t="s">
         <v>81</v>
@@ -818,34 +818,34 @@
         <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="F4" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="G4" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="H4" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="I4" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="J4" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="K4" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="L4" t="s">
         <v>81</v>
@@ -856,34 +856,34 @@
         <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="H5" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="I5" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="J5" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="K5" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="L5" t="s">
         <v>81</v>
@@ -894,34 +894,34 @@
         <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="E6" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="F6" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="G6" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="H6" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="I6" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="J6" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="K6" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="L6" t="s">
         <v>81</v>
@@ -932,34 +932,34 @@
         <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="F7" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="G7" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="H7" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="I7" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="J7" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="K7" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="L7" t="s">
         <v>81</v>
@@ -1014,313 +1014,313 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="F1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="L3" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J4" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="L4" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="K5" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="L5" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="I6" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="K6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="L6" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="J7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="K7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L7" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="G8" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="H8" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="I8" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="J8" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="K8" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="L8" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1656,7 +1656,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1675,28 +1675,28 @@
         <v>83</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="J1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L1" t="s">
         <v>83</v>
@@ -1707,16 +1707,16 @@
         <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F2" t="s">
         <v>87</v>
@@ -1725,16 +1725,16 @@
         <v>87</v>
       </c>
       <c r="H2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L2" t="s">
         <v>83</v>
@@ -1745,16 +1745,16 @@
         <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F3" t="s">
         <v>87</v>
@@ -1763,16 +1763,16 @@
         <v>87</v>
       </c>
       <c r="H3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L3" t="s">
         <v>83</v>
@@ -1783,16 +1783,16 @@
         <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F4" t="s">
         <v>87</v>
@@ -1801,16 +1801,16 @@
         <v>87</v>
       </c>
       <c r="H4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L4" t="s">
         <v>83</v>
@@ -1821,16 +1821,16 @@
         <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
         <v>87</v>
@@ -1839,16 +1839,16 @@
         <v>87</v>
       </c>
       <c r="H5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L5" t="s">
         <v>83</v>
@@ -1859,16 +1859,16 @@
         <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F6" t="s">
         <v>87</v>
@@ -1877,16 +1877,16 @@
         <v>87</v>
       </c>
       <c r="H6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L6" t="s">
         <v>83</v>
@@ -1897,16 +1897,16 @@
         <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F7" t="s">
         <v>87</v>
@@ -1915,16 +1915,16 @@
         <v>87</v>
       </c>
       <c r="H7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L7" t="s">
         <v>83</v>
@@ -1941,28 +1941,28 @@
         <v>83</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="J8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L8" t="s">
         <v>83</v>
@@ -1978,7 +1978,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B2" sqref="B2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2026,34 +2026,34 @@
         <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="H2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="I2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="K2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="L2" t="s">
         <v>84</v>
@@ -2064,34 +2064,34 @@
         <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="F3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="G3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="H3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="I3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="K3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="L3" t="s">
         <v>84</v>
@@ -2178,34 +2178,34 @@
         <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="H6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="I6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="J6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="K6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="L6" t="s">
         <v>84</v>
@@ -2216,34 +2216,34 @@
         <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="H7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="I7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="J7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="K7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="L7" t="s">
         <v>84</v>

</xml_diff>